<commit_message>
Added file by Rayan
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabin\Desktop\2810ICT_PartA-Project-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E439710B-EDED-4F21-84C7-33ADF9C0B19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1A7DD8-61EF-4C80-9CBB-5A33E0DD2970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,90 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>PERIODS</t>
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -231,34 +153,91 @@
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
-  </si>
-  <si>
-    <t>NSW Traffic Penalty Data</t>
+    <t>1.0 Planning</t>
+  </si>
+  <si>
+    <t>1.1 Project plan</t>
+  </si>
+  <si>
+    <t>1.2 Scope</t>
+  </si>
+  <si>
+    <t>1.3 WBS</t>
+  </si>
+  <si>
+    <t>1.4 Activity definition</t>
+  </si>
+  <si>
+    <t>1.5 Scheduling and Gantt chart</t>
+  </si>
+  <si>
+    <t>2.0 Software Design Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2.1 System Vision</t>
+  </si>
+  <si>
+    <t>2.2 Formal requirements</t>
+  </si>
+  <si>
+    <t>2.3 Use cases</t>
+  </si>
+  <si>
+    <t>2.4 Software Design / Components</t>
+  </si>
+  <si>
+    <t>2.5 Interface Design</t>
+  </si>
+  <si>
+    <t>3.0 Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3.1 Test Report</t>
+  </si>
+  <si>
+    <t>3.2 Data processing</t>
+  </si>
+  <si>
+    <t>3.3 User defined data recall</t>
+  </si>
+  <si>
+    <t>3.4 Data visualisation</t>
+  </si>
+  <si>
+    <t>3.5 Gui implementation</t>
+  </si>
+  <si>
+    <t>4.0 Controlling</t>
+  </si>
+  <si>
+    <t>4.1 Progress Meetings</t>
+  </si>
+  <si>
+    <t>4.2 Status reports</t>
+  </si>
+  <si>
+    <t>4.3 Update plans</t>
+  </si>
+  <si>
+    <t>4.4 Update schedual</t>
+  </si>
+  <si>
+    <t>4.5 Version control</t>
+  </si>
+  <si>
+    <t>5.0 Closing</t>
+  </si>
+  <si>
+    <t>5.1 Executive Summary</t>
+  </si>
+  <si>
+    <t>5.2 User Manual</t>
+  </si>
+  <si>
+    <t>5.3 Self Assessment of Schedule</t>
+  </si>
+  <si>
+    <t>Sydney Airbnb Data</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1046,7 @@
   <dimension ref="B1:BO39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1085,7 +1064,7 @@
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
       <c r="B1" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1095,21 +1074,21 @@
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="24" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="30" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1117,21 +1096,21 @@
       <c r="O2" s="32"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="30" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="18"/>
       <c r="V2" s="34" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="W2" s="35"/>
       <c r="X2" s="35"/>
       <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
       <c r="AA2" s="34" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="AB2" s="35"/>
       <c r="AC2" s="35"/>
@@ -1141,7 +1120,7 @@
       <c r="AG2" s="36"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="AJ2" s="23"/>
       <c r="AK2" s="23"/>
@@ -1156,19 +1135,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1383,158 +1362,254 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
+        <v>4</v>
+      </c>
       <c r="G5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2</v>
+      </c>
       <c r="G6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
       <c r="G7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4</v>
+      </c>
+      <c r="E9" s="7">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4</v>
+      </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C10" s="7">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7">
+        <v>4</v>
+      </c>
       <c r="G10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <v>3</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7">
+        <v>4</v>
+      </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <v>4</v>
+      </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>4</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="7">
+        <v>4</v>
+      </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7">
+        <v>4</v>
+      </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="C15" s="9">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7">
+        <v>4</v>
+      </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7">
+        <v>4</v>
+      </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="C17" s="7">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7">
+        <v>7</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8">
@@ -1543,10 +1618,14 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="C18" s="7">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>7</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
@@ -1555,10 +1634,14 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="C19" s="7">
+        <v>5</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8">
@@ -1567,10 +1650,14 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="C20" s="7">
+        <v>7</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
@@ -1579,10 +1666,14 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="C21" s="7">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8">
@@ -1591,10 +1682,14 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C22" s="7">
+        <v>9</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
@@ -1603,82 +1698,98 @@
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>12</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>12</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="8">
-        <v>0</v>
-      </c>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>12</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="8">
-        <v>0</v>
-      </c>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
+        <v>12</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7">
+        <v>12</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="8">
-        <v>0</v>
-      </c>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>12</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="8">
-        <v>0</v>
-      </c>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="C29" s="7">
+        <v>10</v>
+      </c>
+      <c r="D29" s="7">
+        <v>3</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="8">
@@ -1687,10 +1798,14 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="C30" s="7">
+        <v>10</v>
+      </c>
+      <c r="D30" s="7">
+        <v>3</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="8">
@@ -1701,8 +1816,12 @@
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="C31" s="7">
+        <v>10</v>
+      </c>
+      <c r="D31" s="7">
+        <v>3</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="8">
@@ -1713,8 +1832,12 @@
       <c r="B32" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="C32" s="7">
+        <v>12</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="8">
@@ -1722,88 +1845,60 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="8">
-        <v>0</v>
-      </c>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="8">
-        <v>0</v>
-      </c>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="8">
-        <v>0</v>
-      </c>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="8">
-        <v>0</v>
-      </c>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="8">
-        <v>0</v>
-      </c>
+      <c r="G37" s="8"/>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="B38" s="6"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="8">
-        <v>0</v>
-      </c>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="6" t="s">
-        <v>48</v>
-      </c>
+      <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
+      <c r="G39" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1872,7 +1967,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -1882,4 +1977,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c9f92db8-2851-4df9-9d12-fab52f5b1415}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>